<commit_message>
Minor improvements to handmade Model M workbooks.
</commit_message>
<xml_diff>
--- a/ModelM/Handmade/MasterM.xlsx
+++ b/ModelM/Handmade/MasterM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="735"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3825" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3825" uniqueCount="1056">
   <si>
     <t>UNLESS STATED OTHERWISE, THIS WORKBOOK IS ONLY A PROTOTYPE FOR TESTING PURPOSES AND ALL THE DATA IN THIS MODEL ARE FOR ILLUSTRATION ONLY.</t>
   </si>
@@ -3335,6 +3335,15 @@
   </si>
   <si>
     <t>Use copy-paste to replace the entire contents of this sheet with your input data if applicable (data were previously in Calc-Net capex)</t>
+  </si>
+  <si>
+    <t>no company</t>
+  </si>
+  <si>
+    <t>no year</t>
+  </si>
+  <si>
+    <t>no data version</t>
   </si>
 </sst>
 </file>
@@ -4073,37 +4082,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4123,6 +4108,30 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4659,7 +4668,7 @@
   </sheetPr>
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -4671,7 +4680,7 @@
     <row r="1" spans="1:2" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Index for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Index for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Index for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -15895,7 +15904,7 @@
   </sheetPr>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -15907,7 +15916,7 @@
     <row r="1" spans="1:7" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Inputs for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Inputs for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Inputs for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -15941,13 +15950,13 @@
         <v>29</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>33</v>
+        <v>1054</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>33</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -16338,7 +16347,7 @@
     <row r="1" spans="1:8" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Calc-MEAV for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Calc-MEAV for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Calc-MEAV for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="26.25" customHeight="1">
@@ -16474,7 +16483,7 @@
     <row r="1" spans="1:6" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Calc-Units for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Calc-Units for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Calc-Units for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -16713,7 +16722,7 @@
     <row r="1" spans="1:16" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Calc-Net capex for Method M ("&amp;B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Calc-Net capex for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Calc-Net capex for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1">
@@ -16723,21 +16732,21 @@
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
       <c r="D3" s="37"/>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="61" t="s">
         <v>843</v>
       </c>
-      <c r="G3" s="66"/>
-      <c r="H3" s="70"/>
-      <c r="J3" s="65" t="s">
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="J3" s="61" t="s">
         <v>544</v>
       </c>
-      <c r="K3" s="66"/>
-      <c r="L3" s="70"/>
-      <c r="N3" s="72" t="s">
+      <c r="K3" s="62"/>
+      <c r="L3" s="63"/>
+      <c r="N3" s="64" t="s">
         <v>545</v>
       </c>
-      <c r="O3" s="73"/>
-      <c r="P3" s="74"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="66"/>
     </row>
     <row r="4" spans="1:16" ht="12.75" customHeight="1">
       <c r="A4" s="26"/>
@@ -16751,16 +16760,16 @@
       <c r="F4" s="26"/>
       <c r="G4" s="24"/>
       <c r="H4" s="25"/>
-      <c r="J4" s="75" t="s">
+      <c r="J4" s="67" t="s">
         <v>546</v>
       </c>
-      <c r="K4" s="76"/>
-      <c r="L4" s="77"/>
-      <c r="N4" s="75" t="s">
+      <c r="K4" s="68"/>
+      <c r="L4" s="69"/>
+      <c r="N4" s="67" t="s">
         <v>547</v>
       </c>
-      <c r="O4" s="76"/>
-      <c r="P4" s="77"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="69"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="27"/>
@@ -16916,34 +16925,34 @@
     <row r="15" spans="1:16" ht="5.25" customHeight="1"/>
     <row r="16" spans="1:16" ht="26.25" customHeight="1">
       <c r="A16" s="33"/>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="61" t="s">
         <v>847</v>
       </c>
-      <c r="C16" s="70"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="33"/>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="61" t="s">
         <v>848</v>
       </c>
-      <c r="F16" s="70"/>
+      <c r="F16" s="63"/>
       <c r="G16" s="33"/>
-      <c r="H16" s="65" t="s">
+      <c r="H16" s="61" t="s">
         <v>849</v>
       </c>
-      <c r="I16" s="70"/>
+      <c r="I16" s="63"/>
     </row>
     <row r="17" spans="1:9" ht="46" customHeight="1">
       <c r="A17" s="33"/>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="70" t="s">
         <v>850</v>
       </c>
       <c r="C17" s="71"/>
       <c r="D17" s="33"/>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="70" t="s">
         <v>851</v>
       </c>
       <c r="F17" s="71"/>
       <c r="G17" s="33"/>
-      <c r="H17" s="61" t="s">
+      <c r="H17" s="70" t="s">
         <v>852</v>
       </c>
       <c r="I17" s="71"/>
@@ -17049,24 +17058,24 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="33" customFormat="1" ht="37" customHeight="1">
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="61" t="s">
         <v>853</v>
       </c>
-      <c r="C25" s="70"/>
-      <c r="E25" s="67" t="s">
+      <c r="C25" s="63"/>
+      <c r="E25" s="72" t="s">
         <v>854</v>
       </c>
-      <c r="F25" s="68"/>
+      <c r="F25" s="73"/>
     </row>
     <row r="26" spans="1:9" s="33" customFormat="1" ht="27.75" customHeight="1">
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="70" t="s">
         <v>855</v>
       </c>
       <c r="C26" s="71"/>
-      <c r="E26" s="63" t="s">
+      <c r="E26" s="74" t="s">
         <v>856</v>
       </c>
-      <c r="F26" s="64"/>
+      <c r="F26" s="75"/>
     </row>
     <row r="27" spans="1:9">
       <c r="B27" s="26"/>
@@ -17145,37 +17154,37 @@
     </row>
     <row r="35" spans="1:10" ht="5.25" customHeight="1"/>
     <row r="36" spans="1:10" s="33" customFormat="1" ht="51" customHeight="1">
-      <c r="B36" s="65" t="s">
+      <c r="B36" s="61" t="s">
         <v>847</v>
       </c>
-      <c r="C36" s="66"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="38"/>
-      <c r="E36" s="65" t="s">
+      <c r="E36" s="61" t="s">
         <v>848</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="38"/>
-      <c r="H36" s="65" t="s">
+      <c r="H36" s="61" t="s">
         <v>849</v>
       </c>
-      <c r="I36" s="66"/>
+      <c r="I36" s="62"/>
       <c r="J36" s="38"/>
     </row>
     <row r="37" spans="1:10" s="33" customFormat="1" ht="51" customHeight="1">
-      <c r="B37" s="61" t="s">
+      <c r="B37" s="70" t="s">
         <v>850</v>
       </c>
-      <c r="C37" s="62"/>
+      <c r="C37" s="76"/>
       <c r="D37" s="39"/>
-      <c r="E37" s="61" t="s">
+      <c r="E37" s="70" t="s">
         <v>851</v>
       </c>
-      <c r="F37" s="62"/>
+      <c r="F37" s="76"/>
       <c r="G37" s="39"/>
-      <c r="H37" s="61" t="s">
+      <c r="H37" s="70" t="s">
         <v>852</v>
       </c>
-      <c r="I37" s="62"/>
+      <c r="I37" s="76"/>
       <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1">
@@ -17326,35 +17335,35 @@
       <c r="J43" s="29"/>
     </row>
     <row r="46" spans="1:10" s="33" customFormat="1" ht="27.75" customHeight="1">
-      <c r="B46" s="65" t="s">
+      <c r="B46" s="61" t="s">
         <v>853</v>
       </c>
-      <c r="C46" s="66"/>
+      <c r="C46" s="62"/>
       <c r="D46" s="38"/>
-      <c r="E46" s="67" t="s">
+      <c r="E46" s="72" t="s">
         <v>854</v>
       </c>
-      <c r="F46" s="68"/>
-      <c r="H46" s="67" t="s">
+      <c r="F46" s="73"/>
+      <c r="H46" s="72" t="s">
         <v>854</v>
       </c>
-      <c r="I46" s="69"/>
+      <c r="I46" s="77"/>
       <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10" s="33" customFormat="1" ht="27.75" customHeight="1">
-      <c r="B47" s="61" t="s">
+      <c r="B47" s="70" t="s">
         <v>855</v>
       </c>
-      <c r="C47" s="62"/>
+      <c r="C47" s="76"/>
       <c r="D47" s="39"/>
-      <c r="E47" s="63" t="s">
+      <c r="E47" s="74" t="s">
         <v>856</v>
       </c>
-      <c r="F47" s="64"/>
-      <c r="H47" s="61" t="s">
+      <c r="F47" s="75"/>
+      <c r="H47" s="70" t="s">
         <v>859</v>
       </c>
-      <c r="I47" s="62"/>
+      <c r="I47" s="76"/>
       <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
@@ -17764,23 +17773,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="27">
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
     <mergeCell ref="H47:I47"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="E47:F47"/>
@@ -17791,6 +17783,23 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="H46:I46"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17826,7 +17835,7 @@
     <row r="1" spans="1:53" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Calc-Opex for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Calc-Opex for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Calc-Opex for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="3" spans="1:53" ht="58.5" customHeight="1">
@@ -23438,7 +23447,7 @@
     <row r="1" spans="1:9" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Calc-Drivers for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Calc-Drivers for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Calc-Drivers for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" customHeight="1"/>
@@ -23809,7 +23818,7 @@
     <row r="1" spans="1:19" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Calc-Allocation for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Calc-Allocation for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Calc-Allocation for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -25547,7 +25556,7 @@
     <row r="1" spans="1:7" ht="20" customHeight="1">
       <c r="A1" s="4" t="str">
         <f>"Calc-Summary for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Calc-Summary for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Calc-Summary for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14" customHeight="1">
@@ -25816,7 +25825,7 @@
     <row r="1" spans="1:9" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Results for Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Results for Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Results for Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -25964,7 +25973,7 @@
     <row r="1" spans="1:9" ht="19">
       <c r="A1" s="4" t="str">
         <f>"EDCM extension to Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>EDCM extension to Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>EDCM extension to Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -27070,7 +27079,7 @@
     <row r="1" spans="1:9" ht="19">
       <c r="A1" s="4" t="str">
         <f>"Unmetered supplies extension to Method M ("&amp;'Calc-Net capex'!B5&amp;") for "&amp;Inputs!B6&amp;" in "&amp;Inputs!C6&amp;"  Status: "&amp;Inputs!D6&amp;""</f>
-        <v>Unmetered supplies extension to Method M (No option selected) for #VALUE! in #VALUE!  Status: #VALUE!</v>
+        <v>Unmetered supplies extension to Method M (No option selected) for no company in no year  Status: no data version</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>

</xml_diff>

<commit_message>
Correct errors in handmade method M models.
</commit_message>
<xml_diff>
--- a/ModelM/Handmade/MasterM.xlsx
+++ b/ModelM/Handmade/MasterM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="735" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="735"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -3879,7 +3879,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3903,6 +3903,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4140,7 +4144,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="63">
     <cellStyle name="Bad" xfId="11" builtinId="27" hidden="1"/>
     <cellStyle name="Calculation" xfId="15" builtinId="22" hidden="1"/>
     <cellStyle name="Check Cell" xfId="17" builtinId="23" hidden="1"/>
@@ -4184,6 +4188,10 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="10" builtinId="26" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" hidden="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" hidden="1"/>
@@ -4668,7 +4676,7 @@
   </sheetPr>
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -15904,7 +15912,7 @@
   </sheetPr>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -25961,7 +25969,7 @@
   </sheetPr>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A23" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -26786,19 +26794,19 @@
         <v>1000</v>
       </c>
       <c r="B50" s="44" t="e">
-        <f>(SUM('EDCM discounts'!B$28:I$28)-SUMPRODUCT('EDCM discounts'!B41:E41,'EDCM discounts'!F$28:I$28))/(1-SUMPRODUCT('EDCM discounts'!F41:I41,'EDCM discounts'!F$28:I$28))</f>
+        <f>(SUM(B$28:$I$28)-SUMPRODUCT($B41:$E41,$F$28:$I$28))/(1-SUMPRODUCT($F41:$I41,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C50" s="44" t="e">
-        <f>(SUM('EDCM discounts'!C$28:J$28)-SUMPRODUCT('EDCM discounts'!C41:F41,'EDCM discounts'!G$28:J$28))/(1-SUMPRODUCT('EDCM discounts'!G41:J41,'EDCM discounts'!G$28:J$28))</f>
+        <f>(SUM(D$28:$I$28)-SUMPRODUCT($B41:$E41,$F$28:$I$28))/(1-SUM($B$28:C$28)-SUMPRODUCT($F41:$I41,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D50" s="44" t="e">
-        <f>(SUM('EDCM discounts'!D$28:K$28)-SUMPRODUCT('EDCM discounts'!D41:G41,'EDCM discounts'!H$28:K$28))/(1-SUMPRODUCT('EDCM discounts'!H41:K41,'EDCM discounts'!H$28:K$28))</f>
+        <f>(SUM(E$28:$I$28)-SUMPRODUCT($B41:$E41,$F$28:$I$28))/(1-SUM($B$28:D$28)-SUMPRODUCT($F41:$I41,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E50" s="44" t="e">
-        <f>(SUM('EDCM discounts'!E$28:L$28)-SUMPRODUCT('EDCM discounts'!E41:H41,'EDCM discounts'!I$28:L$28))/(1-SUMPRODUCT('EDCM discounts'!I41:L41,'EDCM discounts'!I$28:L$28))</f>
+        <f>(SUM(F$28:$I$28)-SUMPRODUCT($B41:$E41,$F$28:$I$28))/(1-SUM($B$28:E$28)-SUMPRODUCT($F41:$I41,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F50" s="15"/>
@@ -26811,19 +26819,19 @@
         <v>999</v>
       </c>
       <c r="B51" s="44" t="e">
-        <f>(SUM('EDCM discounts'!B$28:I$28)-SUMPRODUCT('EDCM discounts'!B42:E42,'EDCM discounts'!F$28:I$28))/(1-SUMPRODUCT('EDCM discounts'!F42:I42,'EDCM discounts'!F$28:I$28))</f>
+        <f>(SUM(B$28:$I$28)-SUMPRODUCT($B42:$E42,$F$28:$I$28))/(1-SUMPRODUCT($F42:$I42,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C51" s="44" t="e">
-        <f>(SUM('EDCM discounts'!C$28:J$28)-SUMPRODUCT('EDCM discounts'!C42:F42,'EDCM discounts'!G$28:J$28))/(1-SUMPRODUCT('EDCM discounts'!G42:J42,'EDCM discounts'!G$28:J$28))</f>
+        <f>(SUM(D$28:$I$28)-SUMPRODUCT($B42:$E42,$F$28:$I$28))/(1-SUM($B$28:C$28)-SUMPRODUCT($F42:$I42,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D51" s="44" t="e">
-        <f>(SUM('EDCM discounts'!D$28:K$28)-SUMPRODUCT('EDCM discounts'!D42:G42,'EDCM discounts'!H$28:K$28))/(1-SUMPRODUCT('EDCM discounts'!H42:K42,'EDCM discounts'!H$28:K$28))</f>
+        <f>(SUM(E$28:$I$28)-SUMPRODUCT($B42:$E42,$F$28:$I$28))/(1-SUM($B$28:D$28)-SUMPRODUCT($F42:$I42,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E51" s="44" t="e">
-        <f>(SUM('EDCM discounts'!E$28:L$28)-SUMPRODUCT('EDCM discounts'!E42:H42,'EDCM discounts'!I$28:L$28))/(1-SUMPRODUCT('EDCM discounts'!I42:L42,'EDCM discounts'!I$28:L$28))</f>
+        <f>(SUM(F$28:$I$28)-SUMPRODUCT($B42:$E42,$F$28:$I$28))/(1-SUM($B$28:E$28)-SUMPRODUCT($F42:$I42,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F51" s="15"/>
@@ -26836,19 +26844,19 @@
         <v>998</v>
       </c>
       <c r="B52" s="44" t="e">
-        <f>(SUM('EDCM discounts'!B$28:I$28)-SUMPRODUCT('EDCM discounts'!B43:E43,'EDCM discounts'!F$28:I$28))/(1-SUMPRODUCT('EDCM discounts'!F43:I43,'EDCM discounts'!F$28:I$28))</f>
+        <f>(SUM(B$28:$I$28)-SUMPRODUCT($B43:$E43,$F$28:$I$28))/(1-SUMPRODUCT($F43:$I43,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C52" s="44" t="e">
-        <f>(SUM('EDCM discounts'!C$28:J$28)-SUMPRODUCT('EDCM discounts'!C43:F43,'EDCM discounts'!G$28:J$28))/(1-SUMPRODUCT('EDCM discounts'!G43:J43,'EDCM discounts'!G$28:J$28))</f>
+        <f>(SUM(D$28:$I$28)-SUMPRODUCT($B43:$E43,$F$28:$I$28))/(1-SUM($B$28:C$28)-SUMPRODUCT($F43:$I43,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D52" s="44" t="e">
-        <f>(SUM('EDCM discounts'!D$28:K$28)-SUMPRODUCT('EDCM discounts'!D43:G43,'EDCM discounts'!H$28:K$28))/(1-SUMPRODUCT('EDCM discounts'!H43:K43,'EDCM discounts'!H$28:K$28))</f>
+        <f>(SUM(E$28:$I$28)-SUMPRODUCT($B43:$E43,$F$28:$I$28))/(1-SUM($B$28:D$28)-SUMPRODUCT($F43:$I43,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E52" s="44" t="e">
-        <f>(SUM('EDCM discounts'!E$28:L$28)-SUMPRODUCT('EDCM discounts'!E43:H43,'EDCM discounts'!I$28:L$28))/(1-SUMPRODUCT('EDCM discounts'!I43:L43,'EDCM discounts'!I$28:L$28))</f>
+        <f>(SUM(F$28:$I$28)-SUMPRODUCT($B43:$E43,$F$28:$I$28))/(1-SUM($B$28:E$28)-SUMPRODUCT($F43:$I43,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F52" s="15"/>
@@ -26861,19 +26869,19 @@
         <v>997</v>
       </c>
       <c r="B53" s="44" t="e">
-        <f>(SUM('EDCM discounts'!B$28:I$28)-SUMPRODUCT('EDCM discounts'!B44:E44,'EDCM discounts'!F$28:I$28))/(1-SUMPRODUCT('EDCM discounts'!F44:I44,'EDCM discounts'!F$28:I$28))</f>
+        <f>(SUM(B$28:$I$28)-SUMPRODUCT($B44:$E44,$F$28:$I$28))/(1-SUMPRODUCT($F44:$I44,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C53" s="44" t="e">
-        <f>(SUM('EDCM discounts'!C$28:J$28)-SUMPRODUCT('EDCM discounts'!C44:F44,'EDCM discounts'!G$28:J$28))/(1-SUMPRODUCT('EDCM discounts'!G44:J44,'EDCM discounts'!G$28:J$28))</f>
+        <f>(SUM(D$28:$I$28)-SUMPRODUCT($B44:$E44,$F$28:$I$28))/(1-SUM($B$28:C$28)-SUMPRODUCT($F44:$I44,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D53" s="44" t="e">
-        <f>(SUM('EDCM discounts'!D$28:K$28)-SUMPRODUCT('EDCM discounts'!D44:G44,'EDCM discounts'!H$28:K$28))/(1-SUMPRODUCT('EDCM discounts'!H44:K44,'EDCM discounts'!H$28:K$28))</f>
+        <f>(SUM(E$28:$I$28)-SUMPRODUCT($B44:$E44,$F$28:$I$28))/(1-SUM($B$28:D$28)-SUMPRODUCT($F44:$I44,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E53" s="44" t="e">
-        <f>(SUM('EDCM discounts'!E$28:L$28)-SUMPRODUCT('EDCM discounts'!E44:H44,'EDCM discounts'!I$28:L$28))/(1-SUMPRODUCT('EDCM discounts'!I44:L44,'EDCM discounts'!I$28:L$28))</f>
+        <f>(SUM(F$28:$I$28)-SUMPRODUCT($B44:$E44,$F$28:$I$28))/(1-SUM($B$28:E$28)-SUMPRODUCT($F44:$I44,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F53" s="15"/>
@@ -26886,19 +26894,19 @@
         <v>996</v>
       </c>
       <c r="B54" s="44" t="e">
-        <f>(SUM('EDCM discounts'!B$28:I$28)-SUMPRODUCT('EDCM discounts'!B45:E45,'EDCM discounts'!F$28:I$28))/(1-SUMPRODUCT('EDCM discounts'!F45:I45,'EDCM discounts'!F$28:I$28))</f>
+        <f>(SUM(B$28:$I$28)-SUMPRODUCT($B45:$E45,$F$28:$I$28))/(1-SUMPRODUCT($F45:$I45,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C54" s="44" t="e">
-        <f>(SUM('EDCM discounts'!C$28:J$28)-SUMPRODUCT('EDCM discounts'!C45:F45,'EDCM discounts'!G$28:J$28))/(1-SUMPRODUCT('EDCM discounts'!G45:J45,'EDCM discounts'!G$28:J$28))</f>
+        <f>(SUM(D$28:$I$28)-SUMPRODUCT($B45:$E45,$F$28:$I$28))/(1-SUM($B$28:C$28)-SUMPRODUCT($F45:$I45,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D54" s="44" t="e">
-        <f>(SUM('EDCM discounts'!D$28:K$28)-SUMPRODUCT('EDCM discounts'!D45:G45,'EDCM discounts'!H$28:K$28))/(1-SUMPRODUCT('EDCM discounts'!H45:K45,'EDCM discounts'!H$28:K$28))</f>
+        <f>(SUM(E$28:$I$28)-SUMPRODUCT($B45:$E45,$F$28:$I$28))/(1-SUM($B$28:D$28)-SUMPRODUCT($F45:$I45,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E54" s="44" t="e">
-        <f>(SUM('EDCM discounts'!E$28:L$28)-SUMPRODUCT('EDCM discounts'!E45:H45,'EDCM discounts'!I$28:L$28))/(1-SUMPRODUCT('EDCM discounts'!I45:L45,'EDCM discounts'!I$28:L$28))</f>
+        <f>(SUM(F$28:$I$28)-SUMPRODUCT($B45:$E45,$F$28:$I$28))/(1-SUM($B$28:E$28)-SUMPRODUCT($F45:$I45,$F$28:$I$28))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F54" s="15"/>

</xml_diff>